<commit_message>
fixed a precinct header
</commit_message>
<xml_diff>
--- a/MI_Jackson/MI_Jackson_GE20_cleaned.xlsx
+++ b/MI_Jackson/MI_Jackson_GE20_cleaned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITREPOS\gh_kessler\openelections_work\MI_Jackson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C9B706-EB11-40F7-8CB6-29A371B8A64B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E774A9D8-DC2B-4C9B-9400-C40A4E304891}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20360" yWindow="2090" windowWidth="14920" windowHeight="18130" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20360" yWindow="2090" windowWidth="14920" windowHeight="18130" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="total_reg_and_cast" sheetId="2" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="94">
-  <si>
-    <t>Precinct</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="93">
   <si>
     <t>City of Jackson, Ward 1, Precinct 1</t>
   </si>
@@ -712,18 +709,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>1905</v>
@@ -734,7 +731,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2114</v>
@@ -745,7 +742,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1931</v>
@@ -756,7 +753,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>1498</v>
@@ -767,7 +764,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>887</v>
@@ -778,7 +775,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>1758</v>
@@ -789,7 +786,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>1336</v>
@@ -800,7 +797,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>1586</v>
@@ -811,7 +808,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>1373</v>
@@ -822,7 +819,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>1388</v>
@@ -833,7 +830,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>849</v>
@@ -844,7 +841,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>1136</v>
@@ -855,7 +852,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>1274</v>
@@ -866,7 +863,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>1311</v>
@@ -877,7 +874,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>1554</v>
@@ -888,7 +885,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>1560</v>
@@ -899,7 +896,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>2687</v>
@@ -910,7 +907,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>3231</v>
@@ -921,7 +918,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>3364</v>
@@ -932,7 +929,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>3334</v>
@@ -943,7 +940,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>2645</v>
@@ -954,7 +951,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>3300</v>
@@ -965,7 +962,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>1758</v>
@@ -976,7 +973,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>2592</v>
@@ -987,7 +984,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>2192</v>
@@ -998,7 +995,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>2149</v>
@@ -1009,7 +1006,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>1982</v>
@@ -1020,7 +1017,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>916</v>
@@ -1031,7 +1028,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>1356</v>
@@ -1042,7 +1039,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>2050</v>
@@ -1053,7 +1050,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>1782</v>
@@ -1064,7 +1061,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>2111</v>
@@ -1075,7 +1072,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>3252</v>
@@ -1086,7 +1083,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>3149</v>
@@ -1097,7 +1094,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>2638</v>
@@ -1108,7 +1105,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>2373</v>
@@ -1119,7 +1116,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>1582</v>
@@ -1130,7 +1127,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>1112</v>
@@ -1141,7 +1138,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>1967</v>
@@ -1152,7 +1149,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>1768</v>
@@ -1163,7 +1160,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>1980</v>
@@ -1174,7 +1171,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>1066</v>
@@ -1185,7 +1182,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>1405</v>
@@ -1196,7 +1193,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>2353</v>
@@ -1207,7 +1204,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>1484</v>
@@ -1218,7 +1215,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>2237</v>
@@ -1229,7 +1226,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>1601</v>
@@ -1240,7 +1237,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>1340</v>
@@ -1251,7 +1248,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50">
         <v>953</v>
@@ -1262,7 +1259,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <v>876</v>
@@ -1273,7 +1270,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>3038</v>
@@ -1284,7 +1281,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53">
         <v>2786</v>
@@ -1295,7 +1292,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <v>1634</v>
@@ -1306,7 +1303,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <v>2275</v>
@@ -1317,7 +1314,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>2475</v>
@@ -1328,7 +1325,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57">
         <v>2190</v>
@@ -1339,7 +1336,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58">
         <v>2225</v>
@@ -1350,7 +1347,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59">
         <v>2076</v>
@@ -1361,7 +1358,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>1478</v>
@@ -1372,7 +1369,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61">
         <v>2983</v>
@@ -1383,7 +1380,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>2663</v>
@@ -1394,7 +1391,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>2180</v>
@@ -1405,7 +1402,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64">
         <v>2446</v>
@@ -1445,33 +1442,33 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
         <v>66</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>67</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>68</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>70</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>71</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>72</v>
-      </c>
-      <c r="S1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>392</v>
@@ -1497,7 +1494,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>606</v>
@@ -1523,7 +1520,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>253</v>
@@ -1549,7 +1546,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>221</v>
@@ -1575,7 +1572,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>141</v>
@@ -1601,7 +1598,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>297</v>
@@ -1627,7 +1624,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>210</v>
@@ -1653,7 +1650,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>237</v>
@@ -1679,7 +1676,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>214</v>
@@ -1705,7 +1702,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>231</v>
@@ -1731,7 +1728,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>164</v>
@@ -1757,7 +1754,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>192</v>
@@ -1783,7 +1780,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>174</v>
@@ -1809,7 +1806,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>213</v>
@@ -1835,7 +1832,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>282</v>
@@ -1861,7 +1858,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>308</v>
@@ -1887,7 +1884,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>376</v>
@@ -1913,7 +1910,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>410</v>
@@ -1939,7 +1936,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>453</v>
@@ -1965,7 +1962,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>482</v>
@@ -1991,7 +1988,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>359</v>
@@ -2017,7 +2014,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>280</v>
@@ -2043,7 +2040,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>182</v>
@@ -2069,7 +2066,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>288</v>
@@ -2095,7 +2092,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>198</v>
@@ -2121,7 +2118,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>259</v>
@@ -2147,7 +2144,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>281</v>
@@ -2173,7 +2170,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>113</v>
@@ -2199,7 +2196,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>131</v>
@@ -2225,7 +2222,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>119</v>
@@ -2251,7 +2248,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>216</v>
@@ -2277,7 +2274,7 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>275</v>
@@ -2303,7 +2300,7 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>340</v>
@@ -2329,7 +2326,7 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>338</v>
@@ -2355,7 +2352,7 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>299</v>
@@ -2381,7 +2378,7 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>271</v>
@@ -2407,7 +2404,7 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>169</v>
@@ -2433,7 +2430,7 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>106</v>
@@ -2459,7 +2456,7 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>184</v>
@@ -2485,7 +2482,7 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>238</v>
@@ -2511,7 +2508,7 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>197</v>
@@ -2537,7 +2534,7 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>152</v>
@@ -2563,7 +2560,7 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>179</v>
@@ -2589,7 +2586,7 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>209</v>
@@ -2615,7 +2612,7 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>108</v>
@@ -2641,7 +2638,7 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>177</v>
@@ -2667,7 +2664,7 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>136</v>
@@ -2693,7 +2690,7 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>120</v>
@@ -2719,7 +2716,7 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50">
         <v>98</v>
@@ -2745,7 +2742,7 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <v>100</v>
@@ -2771,7 +2768,7 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>251</v>
@@ -2797,7 +2794,7 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53">
         <v>285</v>
@@ -2823,7 +2820,7 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <v>129</v>
@@ -2849,7 +2846,7 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <v>397</v>
@@ -2875,7 +2872,7 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>334</v>
@@ -2901,7 +2898,7 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57">
         <v>358</v>
@@ -2927,7 +2924,7 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58">
         <v>286</v>
@@ -2953,7 +2950,7 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59">
         <v>252</v>
@@ -2979,7 +2976,7 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>206</v>
@@ -3005,7 +3002,7 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61">
         <v>317</v>
@@ -3031,7 +3028,7 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>393</v>
@@ -3057,7 +3054,7 @@
     </row>
     <row r="63" spans="1:19" ht="17" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>191</v>
@@ -3083,7 +3080,7 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64">
         <v>344</v>
@@ -3132,33 +3129,33 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>79</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>80</v>
       </c>
-      <c r="H1" t="s">
-        <v>81</v>
-      </c>
       <c r="I1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>567</v>
@@ -3184,7 +3181,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>763</v>
@@ -3210,7 +3207,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>451</v>
@@ -3236,7 +3233,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>349</v>
@@ -3262,7 +3259,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>199</v>
@@ -3288,7 +3285,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>491</v>
@@ -3314,7 +3311,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>372</v>
@@ -3340,7 +3337,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>423</v>
@@ -3366,7 +3363,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>396</v>
@@ -3392,7 +3389,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>496</v>
@@ -3418,7 +3415,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>240</v>
@@ -3444,7 +3441,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>313</v>
@@ -3470,7 +3467,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>254</v>
@@ -3496,7 +3493,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>539</v>
@@ -3522,7 +3519,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>521</v>
@@ -3548,7 +3545,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>641</v>
@@ -3574,7 +3571,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>601</v>
@@ -3600,7 +3597,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>906</v>
@@ -3626,7 +3623,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>869</v>
@@ -3652,7 +3649,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>849</v>
@@ -3678,7 +3675,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>641</v>
@@ -3704,7 +3701,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>583</v>
@@ -3730,7 +3727,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>475</v>
@@ -3756,7 +3753,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>684</v>
@@ -3782,7 +3779,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>438</v>
@@ -3808,7 +3805,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>604</v>
@@ -3834,7 +3831,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>599</v>
@@ -3860,7 +3857,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>283</v>
@@ -3886,7 +3883,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>287</v>
@@ -3912,7 +3909,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>294</v>
@@ -3938,7 +3935,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>501</v>
@@ -3964,7 +3961,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>471</v>
@@ -3990,7 +3987,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>741</v>
@@ -4016,7 +4013,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>700</v>
@@ -4042,7 +4039,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>633</v>
@@ -4068,7 +4065,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>578</v>
@@ -4094,7 +4091,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>392</v>
@@ -4120,7 +4117,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>271</v>
@@ -4146,7 +4143,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>418</v>
@@ -4172,7 +4169,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>467</v>
@@ -4198,7 +4195,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>482</v>
@@ -4224,7 +4221,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>314</v>
@@ -4250,7 +4247,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>336</v>
@@ -4276,7 +4273,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>460</v>
@@ -4302,7 +4299,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>237</v>
@@ -4328,7 +4325,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>458</v>
@@ -4354,7 +4351,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>372</v>
@@ -4380,7 +4377,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>294</v>
@@ -4406,7 +4403,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50">
         <v>218</v>
@@ -4432,7 +4429,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <v>207</v>
@@ -4458,7 +4455,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>714</v>
@@ -4484,7 +4481,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53">
         <v>711</v>
@@ -4510,7 +4507,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <v>270</v>
@@ -4536,7 +4533,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <v>685</v>
@@ -4562,7 +4559,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>826</v>
@@ -4588,7 +4585,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57">
         <v>801</v>
@@ -4614,7 +4611,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58">
         <v>697</v>
@@ -4640,7 +4637,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59">
         <v>640</v>
@@ -4666,7 +4663,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>466</v>
@@ -4692,7 +4689,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61">
         <v>713</v>
@@ -4718,7 +4715,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>704</v>
@@ -4744,7 +4741,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>403</v>
@@ -4770,7 +4767,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64">
         <v>687</v>
@@ -4822,30 +4819,30 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
         <v>82</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>83</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>84</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>85</v>
       </c>
-      <c r="L1" t="s">
-        <v>86</v>
-      </c>
       <c r="M1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>552</v>
@@ -4868,7 +4865,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>744</v>
@@ -4891,7 +4888,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>442</v>
@@ -4914,7 +4911,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>358</v>
@@ -4937,7 +4934,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>216</v>
@@ -4960,7 +4957,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>527</v>
@@ -4983,7 +4980,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>379</v>
@@ -5006,7 +5003,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>423</v>
@@ -5029,7 +5026,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>401</v>
@@ -5052,7 +5049,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>490</v>
@@ -5075,7 +5072,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>222</v>
@@ -5098,7 +5095,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>317</v>
@@ -5121,7 +5118,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>258</v>
@@ -5144,7 +5141,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>531</v>
@@ -5167,7 +5164,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>518</v>
@@ -5190,7 +5187,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>641</v>
@@ -5213,7 +5210,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>616</v>
@@ -5236,7 +5233,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>911</v>
@@ -5259,7 +5256,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>865</v>
@@ -5282,7 +5279,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>858</v>
@@ -5305,7 +5302,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>655</v>
@@ -5328,7 +5325,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>609</v>
@@ -5351,7 +5348,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>485</v>
@@ -5374,7 +5371,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>689</v>
@@ -5397,7 +5394,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>458</v>
@@ -5420,7 +5417,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>590</v>
@@ -5443,7 +5440,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>612</v>
@@ -5466,7 +5463,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>293</v>
@@ -5489,7 +5486,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>308</v>
@@ -5512,7 +5509,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>325</v>
@@ -5535,7 +5532,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>505</v>
@@ -5558,7 +5555,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>504</v>
@@ -5581,7 +5578,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>768</v>
@@ -5604,7 +5601,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>757</v>
@@ -5627,7 +5624,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>687</v>
@@ -5650,7 +5647,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>615</v>
@@ -5673,7 +5670,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>392</v>
@@ -5696,7 +5693,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>275</v>
@@ -5719,7 +5716,7 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>442</v>
@@ -5742,7 +5739,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>477</v>
@@ -5765,7 +5762,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>489</v>
@@ -5788,7 +5785,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>338</v>
@@ -5811,7 +5808,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>373</v>
@@ -5834,7 +5831,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>477</v>
@@ -5857,7 +5854,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>267</v>
@@ -5880,7 +5877,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>478</v>
@@ -5903,7 +5900,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>380</v>
@@ -5926,7 +5923,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>312</v>
@@ -5949,7 +5946,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50">
         <v>226</v>
@@ -5972,7 +5969,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <v>212</v>
@@ -5995,7 +5992,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>706</v>
@@ -6018,7 +6015,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53">
         <v>712</v>
@@ -6041,7 +6038,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <v>304</v>
@@ -6064,7 +6061,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <v>695</v>
@@ -6087,7 +6084,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>820</v>
@@ -6110,7 +6107,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57">
         <v>778</v>
@@ -6133,7 +6130,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58">
         <v>688</v>
@@ -6156,7 +6153,7 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59">
         <v>598</v>
@@ -6179,7 +6176,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>463</v>
@@ -6202,7 +6199,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61">
         <v>737</v>
@@ -6225,7 +6222,7 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>754</v>
@@ -6248,7 +6245,7 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>437</v>
@@ -6271,7 +6268,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64">
         <v>690</v>
@@ -6301,8 +6298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E2A09D-086C-4398-B448-04CFB5ACCD7A}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -6315,21 +6312,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" t="s">
-        <v>88</v>
-      </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>563</v>
@@ -6343,7 +6340,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>747</v>
@@ -6357,7 +6354,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>439</v>
@@ -6371,7 +6368,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>346</v>
@@ -6385,7 +6382,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>205</v>
@@ -6399,7 +6396,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>487</v>
@@ -6413,7 +6410,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>358</v>
@@ -6427,7 +6424,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>419</v>
@@ -6441,7 +6438,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>379</v>
@@ -6455,7 +6452,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>487</v>
@@ -6469,7 +6466,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>230</v>
@@ -6483,7 +6480,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>310</v>
@@ -6497,7 +6494,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>258</v>
@@ -6511,7 +6508,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>498</v>
@@ -6525,7 +6522,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>513</v>
@@ -6539,7 +6536,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>621</v>
@@ -6553,7 +6550,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>604</v>
@@ -6567,7 +6564,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>857</v>
@@ -6581,7 +6578,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>812</v>
@@ -6595,7 +6592,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>812</v>
@@ -6609,7 +6606,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>638</v>
@@ -6623,7 +6620,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>567</v>
@@ -6637,7 +6634,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>443</v>
@@ -6651,7 +6648,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>632</v>
@@ -6665,7 +6662,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>416</v>
@@ -6679,7 +6676,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>568</v>
@@ -6693,7 +6690,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>591</v>
@@ -6707,7 +6704,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>281</v>
@@ -6721,7 +6718,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>258</v>
@@ -6735,7 +6732,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>289</v>
@@ -6749,7 +6746,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>493</v>
@@ -6763,7 +6760,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>479</v>
@@ -6777,7 +6774,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>727</v>
@@ -6791,7 +6788,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>675</v>
@@ -6805,7 +6802,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>620</v>
@@ -6819,7 +6816,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>568</v>
@@ -6833,7 +6830,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>366</v>
@@ -6847,7 +6844,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>248</v>
@@ -6861,7 +6858,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>400</v>
@@ -6875,7 +6872,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>444</v>
@@ -6889,7 +6886,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>460</v>
@@ -6903,7 +6900,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>302</v>
@@ -6917,7 +6914,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>342</v>
@@ -6931,7 +6928,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>432</v>
@@ -6945,7 +6942,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>223</v>
@@ -6959,7 +6956,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>444</v>
@@ -6973,7 +6970,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>336</v>
@@ -6987,7 +6984,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>277</v>
@@ -7001,7 +6998,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50">
         <v>200</v>
@@ -7015,7 +7012,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <v>194</v>
@@ -7029,7 +7026,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>640</v>
@@ -7043,7 +7040,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53">
         <v>636</v>
@@ -7057,7 +7054,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <v>267</v>
@@ -7071,7 +7068,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <v>664</v>
@@ -7085,7 +7082,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>766</v>
@@ -7099,7 +7096,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57">
         <v>736</v>
@@ -7113,7 +7110,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58">
         <v>637</v>
@@ -7127,7 +7124,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59">
         <v>575</v>
@@ -7141,7 +7138,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>435</v>
@@ -7155,7 +7152,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61">
         <v>679</v>
@@ -7169,7 +7166,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>680</v>
@@ -7183,7 +7180,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>399</v>
@@ -7197,7 +7194,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64">
         <v>678</v>
@@ -7233,24 +7230,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
         <v>89</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>90</v>
       </c>
-      <c r="D1" t="s">
-        <v>91</v>
-      </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>520</v>
@@ -7267,7 +7264,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>732</v>
@@ -7284,7 +7281,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>414</v>
@@ -7301,7 +7298,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>322</v>
@@ -7318,7 +7315,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>188</v>
@@ -7335,7 +7332,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>451</v>
@@ -7352,7 +7349,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>327</v>
@@ -7369,7 +7366,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>385</v>
@@ -7386,7 +7383,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>362</v>
@@ -7403,7 +7400,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>432</v>
@@ -7420,7 +7417,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>227</v>
@@ -7437,7 +7434,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>288</v>
@@ -7454,7 +7451,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>239</v>
@@ -7471,7 +7468,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>465</v>
@@ -7488,7 +7485,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>471</v>
@@ -7505,7 +7502,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>576</v>
@@ -7522,7 +7519,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>346</v>
@@ -7539,7 +7536,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19">
         <v>230</v>
@@ -7556,7 +7553,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20">
         <v>229</v>
@@ -7573,7 +7570,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21">
         <v>339</v>
@@ -7590,7 +7587,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22">
         <v>401</v>
@@ -7607,7 +7604,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>375</v>
@@ -7624,7 +7621,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24">
         <v>373</v>
@@ -7641,7 +7638,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25">
         <v>183</v>
@@ -7658,7 +7655,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26">
         <v>244</v>
@@ -7675,7 +7672,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27">
         <v>165</v>
@@ -7692,7 +7689,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28">
         <v>160</v>
@@ -7709,7 +7706,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29">
         <v>533</v>
@@ -7726,7 +7723,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30">
         <v>551</v>
@@ -7743,7 +7740,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31">
         <v>598</v>
@@ -7760,7 +7757,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32">
         <v>669</v>
@@ -7777,7 +7774,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33">
         <v>663</v>
@@ -7794,7 +7791,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34">
         <v>556</v>
@@ -7811,7 +7808,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35">
         <v>511</v>
@@ -7828,7 +7825,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36">
         <v>379</v>
@@ -7845,7 +7842,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37">
         <v>600</v>
@@ -7862,7 +7859,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38">
         <v>621</v>
@@ -7886,7 +7883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D8C859-4B3B-420F-B1B5-F5D3E8969270}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -7900,21 +7897,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
         <v>92</v>
       </c>
-      <c r="C1" t="s">
-        <v>93</v>
-      </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>584</v>
@@ -7928,7 +7925,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>810</v>
@@ -7942,7 +7939,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>798</v>
@@ -7956,7 +7953,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>796</v>
@@ -7970,7 +7967,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>640</v>
@@ -7984,7 +7981,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>547</v>
@@ -7998,7 +7995,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>424</v>
@@ -8012,7 +8009,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9">
         <v>619</v>
@@ -8026,7 +8023,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>545</v>
@@ -8040,7 +8037,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <v>548</v>
@@ -8054,7 +8051,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>272</v>
@@ -8068,7 +8065,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13">
         <v>452</v>
@@ -8082,7 +8079,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14">
         <v>483</v>
@@ -8096,7 +8093,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15">
         <v>680</v>
@@ -8110,7 +8107,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16">
         <v>652</v>
@@ -8124,7 +8121,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17">
         <v>613</v>
@@ -8138,7 +8135,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>546</v>
@@ -8152,7 +8149,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>358</v>
@@ -8166,7 +8163,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20">
         <v>233</v>
@@ -8180,7 +8177,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21">
         <v>303</v>
@@ -8194,7 +8191,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22">
         <v>318</v>
@@ -8208,7 +8205,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B23">
         <v>390</v>
@@ -8222,7 +8219,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24">
         <v>323</v>
@@ -8236,7 +8233,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25">
         <v>198</v>
@@ -8250,7 +8247,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26">
         <v>363</v>
@@ -8264,7 +8261,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27">
         <v>646</v>

</xml_diff>